<commit_message>
150 questions, solve it daily
</commit_message>
<xml_diff>
--- a/leetcode.xlsx
+++ b/leetcode.xlsx
@@ -14,9 +14,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="47">
-  <si>
-    <t>Array</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="60">
+  <si>
+    <t>`</t>
   </si>
   <si>
     <t>Technique</t>
@@ -207,6 +207,26 @@
     <t xml:space="preserve"> def min_sub_arrayLen(self, target, nums: list): current_sum = 0 , left = 0 , minimum_len = float("inf"). for right in range(len(nums)): current_sum += nums[right] while current_sum &gt;= target: minimum_len = min(minimum_len, right - left + 1) current_sum -= nums[left] return minimum_len if minimum_len != float("inf") else 0</t>
   </si>
   <si>
+    <t>stack</t>
+  </si>
+  <si>
+    <t>20 valid_parentheses</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	stack = []
+	mapping = {'(': ')', '{' : '}', '[' : ']'}		
+	for char in s:
+		if char not in mapping:
+			stack.append(char)
+		else:
+		    if not stack:
+		    	return False
+			top_element = stack.pop()
+			if top_element != mapping[char]
+				return False
+	return not stack</t>
+  </si>
+  <si>
     <t>Two pointers</t>
   </si>
   <si>
@@ -259,6 +279,63 @@
         return True</t>
   </si>
   <si>
+    <t>Matrix</t>
+  </si>
+  <si>
+    <t>36. Valid Sudoku</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        rows = [set() for _ in range(9)]
+        cols = [set() for _ in range(9)]
+        boxes = [set() for _ in range(9)]
+        for i in range(9):
+            for j in range(9):
+                num = board[i][j]
+                if num == '.':
+                    continue
+                box_index = (i // 3) * 3 + (j // 3)
+                if (num in rows[i]) or (num in cols[j]) or (num in boxes[box_index]):
+                    return False
+                rows[i].add(num)
+                cols[j].add(num)
+                boxes[box_index].add(num)
+        return True</t>
+  </si>
+  <si>
+    <t>linkedlist</t>
+  </si>
+  <si>
+    <t>141. Linked List Cycle</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        if not head:
+            return False
+        slow = head
+        fast = head
+        while fast and fast.next:
+            slow = slow.next
+            fast = fast.next.next
+            if slow == fast:
+                return True
+        return False</t>
+  </si>
+  <si>
+    <t>Binary tree</t>
+  </si>
+  <si>
+    <t># 104. Maximum Depth of Binary Tree</t>
+  </si>
+  <si>
+    <t>def maxDepth(self, root: Optional[TreeNode]) -&gt; int:
+	left = maxdepth(root.left) if root else 0
+	right =  maxdepth(root.right) if root else 0
+	depth = max(right, left) + 1 if root else 0
+	return depth</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        </t>
+  </si>
+  <si>
     <t/>
   </si>
   <si>
@@ -273,7 +350,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -299,12 +376,6 @@
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Aptos Narrow"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -335,7 +406,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="11">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -346,25 +417,19 @@
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="4" applyFont="1" fillId="0" quotePrefix="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="4" applyFont="1" fillId="0" quotePrefix="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
@@ -675,14 +740,14 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:B40"/>
+  <dimension ref="A1:B63"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="11" width="56.71928571428572" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="12" width="84.7192857142857" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="9" width="56.71928571428572" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="10" width="84.7192857142857" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="20.25">
@@ -741,16 +806,16 @@
         <v>13</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
       <c r="A8" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="33">
-      <c r="A9" s="6" t="s">
+      <c r="A9" s="5" t="s">
         <v>16</v>
       </c>
       <c r="B9" s="2" t="s">
@@ -766,7 +831,7 @@
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="33">
-      <c r="A11" s="6" t="s">
+      <c r="A11" s="5" t="s">
         <v>20</v>
       </c>
       <c r="B11" s="2" t="s">
@@ -802,7 +867,7 @@
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="433.5">
-      <c r="A17" s="6" t="s">
+      <c r="A17" s="5" t="s">
         <v>25</v>
       </c>
       <c r="B17" s="2" t="s">
@@ -889,67 +954,193 @@
         <v>38</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="18.75" customFormat="1" s="3">
-      <c r="A31" s="2"/>
+    <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="17.25">
+      <c r="A31" s="4"/>
       <c r="B31" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="18.75" customFormat="1" s="3">
-      <c r="A32" s="2"/>
+    <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="17.25">
+      <c r="A32" s="4"/>
       <c r="B32" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="18.75" customFormat="1" s="3">
-      <c r="A33" s="2"/>
+    <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="17.25">
+      <c r="A33" s="4"/>
       <c r="B33" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="18.75" customFormat="1" s="3">
-      <c r="A34" s="2" t="s">
+    <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="17.25">
+      <c r="A34" s="4"/>
+      <c r="B34" s="2"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="17.25">
+      <c r="A35" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="B34" s="2" t="s">
+      <c r="B35" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="128.25">
+      <c r="A36" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="17.25">
+      <c r="A37" s="4"/>
+      <c r="B37" s="2"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="18.75" customFormat="1" s="3">
+      <c r="A38" s="2"/>
+      <c r="B38" s="2"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="18.75" customFormat="1" s="3">
+      <c r="A39" s="2"/>
+      <c r="B39" s="2"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="40" customHeight="1" ht="18.75" customFormat="1" s="3">
+      <c r="A40" s="2"/>
+      <c r="B40" s="2"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="41" customHeight="1" ht="18.75" customFormat="1" s="3">
+      <c r="A41" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B41" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="18.75" customFormat="1" s="3">
-      <c r="A35" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="B35" s="2" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="142.5">
-      <c r="A36" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="B36" s="5" t="s">
+    <row x14ac:dyDescent="0.25" r="42" customHeight="1" ht="18.75" customFormat="1" s="3">
+      <c r="A42" s="2" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="69.75">
-      <c r="A37" s="7" t="s">
+      <c r="B42" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="B37" s="8" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="17.25">
-      <c r="A38" s="9"/>
-      <c r="B38" s="10"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="17.25">
-      <c r="A39" s="9" t="s">
+    </row>
+    <row x14ac:dyDescent="0.25" r="43" customHeight="1" ht="142.5">
+      <c r="A43" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="B39" s="10" t="s">
+      <c r="B43" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="44" customHeight="1" ht="17.25">
+      <c r="A44" s="4"/>
+      <c r="B44" s="2"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="45" customHeight="1" ht="17.25">
+      <c r="A45" s="4"/>
+      <c r="B45" s="2"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="46" customHeight="1" ht="17.25">
+      <c r="A46" s="4"/>
+      <c r="B46" s="2"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="47" customHeight="1" ht="17.25">
+      <c r="A47" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B47" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="40" customHeight="1" ht="18.75" customFormat="1" s="3">
-      <c r="A40" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="B40" s="2"/>
+    <row x14ac:dyDescent="0.25" r="48" customHeight="1" ht="276">
+      <c r="A48" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="49" customHeight="1" ht="17.25">
+      <c r="A49" s="4"/>
+      <c r="B49" s="2"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="50" customHeight="1" ht="17.25">
+      <c r="A50" s="4"/>
+      <c r="B50" s="2"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="51" customHeight="1" ht="17.25">
+      <c r="A51" s="4"/>
+      <c r="B51" s="2"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="52" customHeight="1" ht="17.25">
+      <c r="A52" s="4"/>
+      <c r="B52" s="2"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="53" customHeight="1" ht="17.25">
+      <c r="A53" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="54" customHeight="1" ht="192">
+      <c r="A54" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="55" customHeight="1" ht="17.25">
+      <c r="A55" s="4"/>
+      <c r="B55" s="2"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="56" customHeight="1" ht="17.25">
+      <c r="A56" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="B56" s="7" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="57" customHeight="1" ht="75">
+      <c r="A57" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="B57" s="7" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="58" customHeight="1" ht="17.25">
+      <c r="A58" s="4"/>
+      <c r="B58" s="2"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="59" customHeight="1" ht="17.25">
+      <c r="A59" s="4"/>
+      <c r="B59" s="2"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="60" customHeight="1" ht="69.75">
+      <c r="A60" s="4"/>
+      <c r="B60" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="61" customHeight="1" ht="17.25">
+      <c r="A61" s="4"/>
+      <c r="B61" s="8" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="62" customHeight="1" ht="17.25">
+      <c r="A62" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="B62" s="8" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="63" customHeight="1" ht="18.75" customFormat="1" s="3">
+      <c r="A63" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B63" s="8" t="s">
+        <v>57</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>